<commit_message>
tables and plots for January 2022
</commit_message>
<xml_diff>
--- a/tables/2022-01/regional_table_Jan.xlsx
+++ b/tables/2022-01/regional_table_Jan.xlsx
@@ -122,7 +122,7 @@
     <t>-</t>
   </si>
   <si>
-    <t>6.3 (5.8-6.7)</t>
+    <t>6.2 (5.8-6.7)</t>
   </si>
   <si>
     <t>5.4 (4.6-6.2)</t>
@@ -149,10 +149,10 @@
     <t>93.7 (92.8-94.5)</t>
   </si>
   <si>
-    <t>89.7 (88.1-91.1)</t>
-  </si>
-  <si>
-    <t>91.6 (90.6-92.6)</t>
+    <t>89.7 (88.2-91.1)</t>
+  </si>
+  <si>
+    <t>91.7 (90.6-92.6)</t>
   </si>
   <si>
     <t>90.0 (87.0-92.5)</t>
@@ -301,7 +301,7 @@
         <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>11272.0</v>
+        <v>11287.0</v>
       </c>
       <c r="C2" t="s">
         <v>27</v>
@@ -349,7 +349,7 @@
         <v>35</v>
       </c>
       <c r="R2" t="n">
-        <v>10360.0</v>
+        <v>10375.0</v>
       </c>
       <c r="S2" t="s">
         <v>43</v>
@@ -366,7 +366,7 @@
         <v>21</v>
       </c>
       <c r="B3" t="n">
-        <v>3310.0</v>
+        <v>3316.0</v>
       </c>
       <c r="C3" t="s">
         <v>27</v>
@@ -414,7 +414,7 @@
         <v>35</v>
       </c>
       <c r="R3" t="n">
-        <v>3100.0</v>
+        <v>3106.0</v>
       </c>
       <c r="S3" t="s">
         <v>44</v>
@@ -431,7 +431,7 @@
         <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>1653.0</v>
+        <v>1655.0</v>
       </c>
       <c r="C4" t="s">
         <v>28</v>
@@ -479,7 +479,7 @@
         <v>35</v>
       </c>
       <c r="R4" t="n">
-        <v>1483.0</v>
+        <v>1485.0</v>
       </c>
       <c r="S4" t="s">
         <v>45</v>
@@ -496,7 +496,7 @@
         <v>23</v>
       </c>
       <c r="B5" t="n">
-        <v>2922.0</v>
+        <v>2925.0</v>
       </c>
       <c r="C5" t="s">
         <v>29</v>
@@ -544,7 +544,7 @@
         <v>35</v>
       </c>
       <c r="R5" t="n">
-        <v>2678.0</v>
+        <v>2681.0</v>
       </c>
       <c r="S5" t="s">
         <v>46</v>
@@ -626,7 +626,7 @@
         <v>25</v>
       </c>
       <c r="B7" t="n">
-        <v>2038.0</v>
+        <v>2042.0</v>
       </c>
       <c r="C7" t="s">
         <v>31</v>
@@ -674,7 +674,7 @@
         <v>35</v>
       </c>
       <c r="R7" t="n">
-        <v>1860.0</v>
+        <v>1864.0</v>
       </c>
       <c r="S7" t="s">
         <v>48</v>

</xml_diff>